<commit_message>
avances plan de prueba
</commit_message>
<xml_diff>
--- a/Fase 2/Plan de Pruebas.xlsx
+++ b/Fase 2/Plan de Pruebas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E2EF76-A076-4948-A56B-DAF33B67F2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8A5117-CF0D-493F-9AF7-887AB1593C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2160" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
   <si>
     <t>Caso de Prueba</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>CP-012</t>
-  </si>
-  <si>
-    <t>CP-013</t>
   </si>
   <si>
     <t>CP-014</t>
@@ -259,21 +256,13 @@
 5. Verificar que las licitaciones no relacionadas no se muestren en los resultados.</t>
   </si>
   <si>
-    <t>1. Logear correctamente para que se redirija al page del dashboard
-2. Revisar que los gráficos y tablas que presentan estadísticas de las licitaciones con seguimiento se carguen correctamente.
-3. Verificar que los datos mostrados coincidan con la información de licitaciones activas y sean consistentes con el backend o base de datos.
-4. Actualizar la página del dashboard y confirmar que los datos se refrescan correctamente sin pérdida de información.</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
     <t xml:space="preserve"> El sistema debe permitir iniciar sesión con correo y contraseña, mostrar/ocultar la contraseña, y manejar errores de autenticación.</t>
   </si>
   <si>
-    <t>Login exitoso: El usuario es redirigido a la página principal y se muestra un mensaje de bienvenida personalizado que indica que ha iniciado sesión correctamente.
-Login fallido: El sistema muestra un mensaje de error claro que indica que las credenciales son incorrectas y permanece en la página de login sin redirigir al usuario.
-Mostrar/Ocultar contraseña: La contraseña se muestra o se oculta según la acción del usuario, y el ícono cambia de estado de acuerdo con la acción realizada.</t>
+    <t>CP-015</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -281,12 +270,25 @@
 1. Ingresar correo nico.vidal.m@gmail.com y contraseña válidos n1234567.
 2. Hacer clic en "Iniciar sesión".
 3. Verificar redirección a la página principal.
-Login fallido:
-1. Ingresar credenciales incorrectas.
-.2. Verificar mensaje de error "Correo o contraseña incorrectos".
-Mostrar/Ocultar contraseña:
-1. Hacer clic en el ícono de mostrar/ocultar contraseña.
-2. Verificar que se muestra/oculta correctamente.</t>
+</t>
+  </si>
+  <si>
+    <t>Login exitoso</t>
+  </si>
+  <si>
+    <t>Completado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login exitoso: El usuario es redirigido a la página principal y se muestra un mensaje de bienvenida personalizado que indica que ha iniciado sesión correctamente.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar correo nico.vidal.m@gmail.com y contraseña válidos n1234567.
+2.diriga hacia dashboard y carguen los diferentes cuadros con datos
+</t>
+  </si>
+  <si>
+    <t>Obtencion exitosa</t>
   </si>
 </sst>
 </file>
@@ -442,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -484,6 +486,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -792,8 +797,8 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,88 +839,96 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="264" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>9</v>
+      <c r="B2" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="D2" s="16">
+        <v>45578</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="H2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>10</v>
+      <c r="B3" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6" t="s">
-        <v>48</v>
+        <v>21</v>
+      </c>
+      <c r="D3" s="16">
+        <v>45581</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="H3" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>11</v>
+      <c r="B4" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>24</v>
+      <c r="B5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="5" t="s">
@@ -926,15 +939,15 @@
       <c r="A6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>25</v>
+      <c r="B6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>67</v>
@@ -944,22 +957,22 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>26</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>25</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5" t="s">
@@ -971,17 +984,17 @@
         <v>39</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="5" t="s">
@@ -993,13 +1006,19 @@
         <v>40</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="11"/>
+        <v>15</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="E9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="6"/>
       <c r="H9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1009,83 +1028,77 @@
         <v>41</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>28</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C10" s="11"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="264" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5" t="s">
@@ -1104,10 +1117,10 @@
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
@@ -1116,7 +1129,7 @@
     </row>
     <row r="15" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>20</v>
@@ -1126,10 +1139,10 @@
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5" t="s">

</xml_diff>

<commit_message>
Avance plan de pruebas
</commit_message>
<xml_diff>
--- a/Fase 2/Plan de Pruebas.xlsx
+++ b/Fase 2/Plan de Pruebas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8A5117-CF0D-493F-9AF7-887AB1593C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B68DFE-F2E2-43CC-8F3B-BB2439831CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2160" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
   <si>
     <t>Caso de Prueba</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Cuenta page con datos del usuario</t>
   </si>
   <si>
-    <t>Scroll de oportunidades en seguimiento</t>
-  </si>
-  <si>
     <t>Usar BottomNavigator</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Ver item de las oportunidades</t>
   </si>
   <si>
-    <t>Email no editable en page cuenta</t>
-  </si>
-  <si>
     <t xml:space="preserve">Crear cuenta </t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>Debe haber un page llamado "Cuenta" donde el usuario pueda visualizar sus datos.</t>
   </si>
   <si>
-    <t>Debe existir un scroll en las oportunidades de seguimientos para poder visualizar más oportunidades.</t>
-  </si>
-  <si>
     <t>El sistema de navegacion de la aplicación debe ser un BottomNavigator.</t>
   </si>
   <si>
@@ -107,15 +98,6 @@
     <t>Boton en el login con iconos para mostrar y ocultar la contraseña.</t>
   </si>
   <si>
-    <t>El email que se visualizará en el page 'Cuenta', no debe ser modificable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> El login debe poseer un boton que redireccione a la pagina web para crear una cuenta de usuario.</t>
-  </si>
-  <si>
-    <t>La aplicación debe poseer un boton para deslogear.</t>
-  </si>
-  <si>
     <t>CP-001</t>
   </si>
   <si>
@@ -170,12 +152,6 @@
     <t xml:space="preserve"> La página "Cuenta" debe mostrar correctamente los datos personales del usuario (nombre, email, etc.).</t>
   </si>
   <si>
-    <t xml:space="preserve"> El usuario debe poder hacer scroll para ver todas las oportunidades en seguimiento sin interrupciones</t>
-  </si>
-  <si>
-    <t>1. Navegar a la pantalla de seguimiento. 2. Hacer scroll en la lista de oportunidades. 3. Verificar que el scroll funcione sin problemas.</t>
-  </si>
-  <si>
     <t>El sistema de navegación debe funcionar con un BottomNavigator que permita moverse entre las diferentes secciones de la aplicación (Home, Seguimiento, Cuenta).</t>
   </si>
   <si>
@@ -183,15 +159,6 @@
   </si>
   <si>
     <t xml:space="preserve"> En la página de login, debería haber un botón para mostrar u ocultar la contraseña mediante íconos.</t>
-  </si>
-  <si>
-    <t>El correo electrónico mostrado en la página de "Cuenta" no debe ser editable.</t>
-  </si>
-  <si>
-    <t>El botón en el login debería redirigir a una página donde el usuario pueda crear una cuenta nueva.</t>
-  </si>
-  <si>
-    <t>El sistema debería permitir que el usuario cierre sesión mediante un botón visible para desloguearse.</t>
   </si>
   <si>
     <t>5.1. Ingresar a la página de seguimiento desde el menú de navegación principal.
@@ -213,25 +180,6 @@
 2.3. Verificar que el sistema guarda y muestra el nombre actualizado.</t>
   </si>
   <si>
-    <t xml:space="preserve">Registro exitoso:
-1.1. Navegar a la pantalla "Crear cuenta".
-1.2. Ingresar nombre, correo electrónico y contraseña válidos.
-1.3. Hacer clic en "Registrar".
-1.4. Verificar que el sistema redirige a la página principal con el usuario registrado.
-.
-</t>
-  </si>
-  <si>
-    <t>Logout exitoso:
-1.1. Navegar a la opción "Cerrar sesión" en el menú de usuario.
-1.2. Hacer clic en "Logout".
-1.3. Verificar que el sistema redirige a la página de login o inicio.</t>
-  </si>
-  <si>
-    <t>1. Intentar hacer clic o modificar el campo de correo electrónico en la página de cuenta.
-2. Confirmar que el campo de correo no sea editable y que la aplicación lo maneje correctamente.</t>
-  </si>
-  <si>
     <t>1. Hacer clic en el módulo de oportunidades en la sección de seguimiento.
 2. Verificar que se muestren todos los ítems relacionados con las diferentes oportunidades de negocio.</t>
   </si>
@@ -260,9 +208,6 @@
   </si>
   <si>
     <t xml:space="preserve"> El sistema debe permitir iniciar sesión con correo y contraseña, mostrar/ocultar la contraseña, y manejar errores de autenticación.</t>
-  </si>
-  <si>
-    <t>CP-015</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -288,7 +233,77 @@
 </t>
   </si>
   <si>
-    <t>Obtencion exitosa</t>
+    <t>LoginFail</t>
+  </si>
+  <si>
+    <t>El sistema debe mostrar un mensaje de error cuando se intenta iniciar sesión con credenciales inválidas.</t>
+  </si>
+  <si>
+    <t>Error en el inicio de sesión: El usuario ve un mensaje de error indicando que el correo o la contraseña son incorrectos</t>
+  </si>
+  <si>
+    <t>1. Ingresar correo "wrong.email@example.com" y contraseña inválida "wrongpassword".
+2. Hacer clic en "Iniciar sesión".
+3. Verificar que se muestra el mensaje de error.</t>
+  </si>
+  <si>
+    <t>Mensaje de error mostrado</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario acceder a la opción de registro desde la pantalla de login.</t>
+  </si>
+  <si>
+    <t>El usuario hace clic en el botón "Registrate aquí" y es dirigido a la pagina de registro.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registro exitoso:
+1.0. Hacer click en "Registrate aquí"
+1.1. Ser redirigido a la pantalla "Crear cuenta".
+1.2. Ingresar nombre, correo electrónico y contraseña válidos.
+1.3. Hacer clic en "Registrar".
+1.4. Verificar que el sistema redirige a la página principal con el usuario registrado.
+.
+</t>
+  </si>
+  <si>
+    <t>Pantalla de registro mostrada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recuperación de Contraseña </t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario acceder a la opción de recuperación de contraseña desde la pantalla login.</t>
+  </si>
+  <si>
+    <t>El usuario hace clic en "¿Olvidaste tu Contraseña" y es redirigido a la página de recuperación de contraseña.</t>
+  </si>
+  <si>
+    <t>1.0. Hacer click en  "¿Olvidaste tu Contraseña"
+1.1. Ser redirigido a la página "Crear cuenta".
+1.2. Ingresar nombre, correo electrónico y contraseña válidos.
+1.3. Hacer clic en "Continuar".
+1.4. Verificar que el sistema redirige a la página principal con el usuario registrado.</t>
+  </si>
+  <si>
+    <t>Pantalla de recuperación de contraseña mostrada</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario cerrar sesión desde la pantalla principal después de haber iniciado sesión.</t>
+  </si>
+  <si>
+    <t>El usuario hace clic en "Logout" y es dirigido nuevamente a la pantalla de inicio de sesión</t>
+  </si>
+  <si>
+    <t>Logout exitoso:
+1.0. Logear correctamente
+1.1. Hacer click en el boton "Cerrar sesión" 
+1.2. Verificar que el sistema redirige a la página de login o inicio.</t>
+  </si>
+  <si>
+    <t>Redirigido a la pantalla de inicio de sesión</t>
+  </si>
+  <si>
+    <t>CP-013</t>
   </si>
 </sst>
 </file>
@@ -796,9 +811,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,160 +856,174 @@
     </row>
     <row r="2" spans="1:8" ht="264" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D2" s="16">
         <v>45578</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="D3" s="16">
-        <v>45581</v>
+        <v>45578</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="D4" s="16">
+        <v>45578</v>
+      </c>
       <c r="E4" s="6" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="H4" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="D5" s="16">
+        <v>45578</v>
+      </c>
       <c r="E5" s="6" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="D6" s="16">
+        <v>45579</v>
+      </c>
       <c r="E6" s="6" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="H6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="D7" s="16">
+        <v>45581</v>
+      </c>
       <c r="E7" s="6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="5" t="s">
@@ -1003,20 +1032,20 @@
     </row>
     <row r="9" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="5" t="s">
@@ -1025,15 +1054,21 @@
     </row>
     <row r="10" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
         <v>8</v>
@@ -1041,20 +1076,20 @@
     </row>
     <row r="11" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5" t="s">
@@ -1063,20 +1098,20 @@
     </row>
     <row r="12" spans="1:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5" t="s">
@@ -1085,21 +1120,15 @@
     </row>
     <row r="13" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>30</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C13" s="11"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5" t="s">
         <v>8</v>
@@ -1107,20 +1136,20 @@
     </row>
     <row r="14" spans="1:8" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
@@ -1129,20 +1158,20 @@
     </row>
     <row r="15" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="8" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5" t="s">

</xml_diff>

<commit_message>
Avance plan de pruebas 2
</commit_message>
<xml_diff>
--- a/Fase 2/Plan de Pruebas.xlsx
+++ b/Fase 2/Plan de Pruebas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D944D8F-A122-44E3-BEBB-52EA243B5FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B68DFE-F2E2-43CC-8F3B-BB2439831CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2160" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
   <si>
     <t>Caso de Prueba</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Cuenta page con datos del usuario</t>
   </si>
   <si>
-    <t>Scroll de oportunidades en seguimiento</t>
-  </si>
-  <si>
     <t>Usar BottomNavigator</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Ver item de las oportunidades</t>
   </si>
   <si>
-    <t>Email no editable en page cuenta</t>
-  </si>
-  <si>
     <t xml:space="preserve">Crear cuenta </t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>Debe haber un page llamado "Cuenta" donde el usuario pueda visualizar sus datos.</t>
   </si>
   <si>
-    <t>Debe existir un scroll en las oportunidades de seguimientos para poder visualizar más oportunidades.</t>
-  </si>
-  <si>
     <t>El sistema de navegacion de la aplicación debe ser un BottomNavigator.</t>
   </si>
   <si>
@@ -107,15 +98,6 @@
     <t>Boton en el login con iconos para mostrar y ocultar la contraseña.</t>
   </si>
   <si>
-    <t>El email que se visualizará en el page 'Cuenta', no debe ser modificable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> El login debe poseer un boton que redireccione a la pagina web para crear una cuenta de usuario.</t>
-  </si>
-  <si>
-    <t>La aplicación debe poseer un boton para deslogear.</t>
-  </si>
-  <si>
     <t>CP-001</t>
   </si>
   <si>
@@ -152,9 +134,6 @@
     <t>CP-012</t>
   </si>
   <si>
-    <t>CP-013</t>
-  </si>
-  <si>
     <t>CP-014</t>
   </si>
   <si>
@@ -173,12 +152,6 @@
     <t xml:space="preserve"> La página "Cuenta" debe mostrar correctamente los datos personales del usuario (nombre, email, etc.).</t>
   </si>
   <si>
-    <t xml:space="preserve"> El usuario debe poder hacer scroll para ver todas las oportunidades en seguimiento sin interrupciones</t>
-  </si>
-  <si>
-    <t>1. Navegar a la pantalla de seguimiento. 2. Hacer scroll en la lista de oportunidades. 3. Verificar que el scroll funcione sin problemas.</t>
-  </si>
-  <si>
     <t>El sistema de navegación debe funcionar con un BottomNavigator que permita moverse entre las diferentes secciones de la aplicación (Home, Seguimiento, Cuenta).</t>
   </si>
   <si>
@@ -186,15 +159,6 @@
   </si>
   <si>
     <t xml:space="preserve"> En la página de login, debería haber un botón para mostrar u ocultar la contraseña mediante íconos.</t>
-  </si>
-  <si>
-    <t>El correo electrónico mostrado en la página de "Cuenta" no debe ser editable.</t>
-  </si>
-  <si>
-    <t>El botón en el login debería redirigir a una página donde el usuario pueda crear una cuenta nueva.</t>
-  </si>
-  <si>
-    <t>El sistema debería permitir que el usuario cierre sesión mediante un botón visible para desloguearse.</t>
   </si>
   <si>
     <t>5.1. Ingresar a la página de seguimiento desde el menú de navegación principal.
@@ -216,8 +180,85 @@
 2.3. Verificar que el sistema guarda y muestra el nombre actualizado.</t>
   </si>
   <si>
+    <t>1. Hacer clic en el módulo de oportunidades en la sección de seguimiento.
+2. Verificar que se muestren todos los ítems relacionados con las diferentes oportunidades de negocio.</t>
+  </si>
+  <si>
+    <t>1. Navegar a la sección "Cuenta" desde el menú principal de la aplicación.
+2. Verificar que los datos del usuario, como nombre, correo electrónico, y otra información personal, se muestren correctamente.
+3. Probar editar algunos de los datos personales (como cambiar el correo electrónico) y confirmar que los cambios se guardan correctamente.
+.4. Cerrar sesión y volver a iniciar para comprobar que los datos actualizados se mantengan.
+.5. Verificar que no se muestren datos de otros usuarios por error.</t>
+  </si>
+  <si>
+    <t>1. En la sección de seguimiento, aplicar el filtro por "Estado de oportunidad" (por ejemplo, Compra Ágil, Cotizaciones).
+.2. Verificar que solo las licitaciones que corresponden a ese estado se muestren en la lista, y que el resto de las licitaciones no se visualicen.
+3. Cambiar el filtro varias veces entre los diferentes estados de oportunidad y verificar que los resultados cambian correctamente sin errores.
+4. Verificar que los datos dentro de cada licitación (como fechas y descripción) coincidan con el estado filtrado.</t>
+  </si>
+  <si>
+    <t>.1 Desde la pantalla principal, navegar a la sección de seguimiento de licitaciones.
+2. En el campo de búsqueda, ingresar palabras clave relacionadas con licitaciones que deberían estar registradas (ej. "Compra", "Proyecto").
+3. Verificar que las licitaciones que coinciden con las palabras ingresadas se filtren correctamente y se muestren sin errores.
+4. Probar búsquedas con diferentes criterios (por ejemplo, palabras incompletas o errores tipográficos) para verificar si la búsqueda es tolerante a errores o necesita mejoras.
+5. Verificar que las licitaciones no relacionadas no se muestren en los resultados.</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El sistema debe permitir iniciar sesión con correo y contraseña, mostrar/ocultar la contraseña, y manejar errores de autenticación.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Login exitoso:
+1. Ingresar correo nico.vidal.m@gmail.com y contraseña válidos n1234567.
+2. Hacer clic en "Iniciar sesión".
+3. Verificar redirección a la página principal.
+</t>
+  </si>
+  <si>
+    <t>Login exitoso</t>
+  </si>
+  <si>
+    <t>Completado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login exitoso: El usuario es redirigido a la página principal y se muestra un mensaje de bienvenida personalizado que indica que ha iniciado sesión correctamente.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar correo nico.vidal.m@gmail.com y contraseña válidos n1234567.
+2.diriga hacia dashboard y carguen los diferentes cuadros con datos
+</t>
+  </si>
+  <si>
+    <t>LoginFail</t>
+  </si>
+  <si>
+    <t>El sistema debe mostrar un mensaje de error cuando se intenta iniciar sesión con credenciales inválidas.</t>
+  </si>
+  <si>
+    <t>Error en el inicio de sesión: El usuario ve un mensaje de error indicando que el correo o la contraseña son incorrectos</t>
+  </si>
+  <si>
+    <t>1. Ingresar correo "wrong.email@example.com" y contraseña inválida "wrongpassword".
+2. Hacer clic en "Iniciar sesión".
+3. Verificar que se muestra el mensaje de error.</t>
+  </si>
+  <si>
+    <t>Mensaje de error mostrado</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario acceder a la opción de registro desde la pantalla de login.</t>
+  </si>
+  <si>
+    <t>El usuario hace clic en el botón "Registrate aquí" y es dirigido a la pagina de registro.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Registro exitoso:
-1.1. Navegar a la pantalla "Crear cuenta".
+1.0. Hacer click en "Registrate aquí"
+1.1. Ser redirigido a la pantalla "Crear cuenta".
 1.2. Ingresar nombre, correo electrónico y contraseña válidos.
 1.3. Hacer clic en "Registrar".
 1.4. Verificar que el sistema redirige a la página principal con el usuario registrado.
@@ -225,68 +266,44 @@
 </t>
   </si>
   <si>
+    <t>Pantalla de registro mostrada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recuperación de Contraseña </t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario acceder a la opción de recuperación de contraseña desde la pantalla login.</t>
+  </si>
+  <si>
+    <t>El usuario hace clic en "¿Olvidaste tu Contraseña" y es redirigido a la página de recuperación de contraseña.</t>
+  </si>
+  <si>
+    <t>1.0. Hacer click en  "¿Olvidaste tu Contraseña"
+1.1. Ser redirigido a la página "Crear cuenta".
+1.2. Ingresar nombre, correo electrónico y contraseña válidos.
+1.3. Hacer clic en "Continuar".
+1.4. Verificar que el sistema redirige a la página principal con el usuario registrado.</t>
+  </si>
+  <si>
+    <t>Pantalla de recuperación de contraseña mostrada</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario cerrar sesión desde la pantalla principal después de haber iniciado sesión.</t>
+  </si>
+  <si>
+    <t>El usuario hace clic en "Logout" y es dirigido nuevamente a la pantalla de inicio de sesión</t>
+  </si>
+  <si>
     <t>Logout exitoso:
-1.1. Navegar a la opción "Cerrar sesión" en el menú de usuario.
-1.2. Hacer clic en "Logout".
-1.3. Verificar que el sistema redirige a la página de login o inicio.</t>
-  </si>
-  <si>
-    <t>1. Intentar hacer clic o modificar el campo de correo electrónico en la página de cuenta.
-2. Confirmar que el campo de correo no sea editable y que la aplicación lo maneje correctamente.</t>
-  </si>
-  <si>
-    <t>1. Hacer clic en el módulo de oportunidades en la sección de seguimiento.
-2. Verificar que se muestren todos los ítems relacionados con las diferentes oportunidades de negocio.</t>
-  </si>
-  <si>
-    <t>1. Navegar a la sección "Cuenta" desde el menú principal de la aplicación.
-2. Verificar que los datos del usuario, como nombre, correo electrónico, y otra información personal, se muestren correctamente.
-3. Probar editar algunos de los datos personales (como cambiar el correo electrónico) y confirmar que los cambios se guardan correctamente.
-.4. Cerrar sesión y volver a iniciar para comprobar que los datos actualizados se mantengan.
-.5. Verificar que no se muestren datos de otros usuarios por error.</t>
-  </si>
-  <si>
-    <t>1. En la sección de seguimiento, aplicar el filtro por "Estado de oportunidad" (por ejemplo, Compra Ágil, Cotizaciones).
-.2. Verificar que solo las licitaciones que corresponden a ese estado se muestren en la lista, y que el resto de las licitaciones no se visualicen.
-3. Cambiar el filtro varias veces entre los diferentes estados de oportunidad y verificar que los resultados cambian correctamente sin errores.
-4. Verificar que los datos dentro de cada licitación (como fechas y descripción) coincidan con el estado filtrado.</t>
-  </si>
-  <si>
-    <t>.1 Desde la pantalla principal, navegar a la sección de seguimiento de licitaciones.
-2. En el campo de búsqueda, ingresar palabras clave relacionadas con licitaciones que deberían estar registradas (ej. "Compra", "Proyecto").
-3. Verificar que las licitaciones que coinciden con las palabras ingresadas se filtren correctamente y se muestren sin errores.
-4. Probar búsquedas con diferentes criterios (por ejemplo, palabras incompletas o errores tipográficos) para verificar si la búsqueda es tolerante a errores o necesita mejoras.
-5. Verificar que las licitaciones no relacionadas no se muestren en los resultados.</t>
-  </si>
-  <si>
-    <t>1. Logear correctamente para que se redirija al page del dashboard
-2. Revisar que los gráficos y tablas que presentan estadísticas de las licitaciones con seguimiento se carguen correctamente.
-3. Verificar que los datos mostrados coincidan con la información de licitaciones activas y sean consistentes con el backend o base de datos.
-4. Actualizar la página del dashboard y confirmar que los datos se refrescan correctamente sin pérdida de información.</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> El sistema debe permitir iniciar sesión con correo y contraseña,.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login exitoso: El usuario es redirigido a la página principal y se muestra un mensaje de bienvenida personalizado que indica que ha iniciado sesión correctamente.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Login exitoso:
-1. Ingresar correo nico.vidal.m@gmail.com y contraseña válidos n1234567.
-2. Hacer clic en "Iniciar sesión".
-3. Verificar redirección a la página principal de dashboard
-</t>
-  </si>
-  <si>
-    <t>Existoso</t>
-  </si>
-  <si>
-    <t>Completado</t>
+1.0. Logear correctamente
+1.1. Hacer click en el boton "Cerrar sesión" 
+1.2. Verificar que el sistema redirige a la página de login o inicio.</t>
+  </si>
+  <si>
+    <t>Redirigido a la pantalla de inicio de sesión</t>
+  </si>
+  <si>
+    <t>CP-013</t>
   </si>
 </sst>
 </file>
@@ -794,9 +811,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,158 +854,176 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="264" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D2" s="16">
         <v>45578</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="D3" s="16">
+        <v>45578</v>
+      </c>
       <c r="E3" s="8" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="6"/>
+        <v>65</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="H3" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="D4" s="16">
+        <v>45578</v>
+      </c>
       <c r="E4" s="6" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="H4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="D5" s="16">
+        <v>45578</v>
+      </c>
       <c r="E5" s="6" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="6"/>
+        <v>74</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="H5" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="D6" s="16">
+        <v>45579</v>
+      </c>
       <c r="E6" s="6" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="H6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="D7" s="16">
+        <v>45581</v>
+      </c>
       <c r="E7" s="6" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="5" t="s">
@@ -997,20 +1032,20 @@
     </row>
     <row r="9" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="5" t="s">
@@ -1019,81 +1054,81 @@
     </row>
     <row r="10" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="264" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>30</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C13" s="11"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5" t="s">
         <v>8</v>
@@ -1101,20 +1136,20 @@
     </row>
     <row r="14" spans="1:8" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
@@ -1123,20 +1158,20 @@
     </row>
     <row r="15" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="8" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5" t="s">

</xml_diff>

<commit_message>
Plan de pruebas 9
</commit_message>
<xml_diff>
--- a/Fase 2/Plan de Pruebas.xlsx
+++ b/Fase 2/Plan de Pruebas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B68DFE-F2E2-43CC-8F3B-BB2439831CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B4FF7F-B57A-4096-A656-F323ABB20F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
   <si>
     <t>Caso de Prueba</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Busqueda en seguimiento</t>
   </si>
   <si>
-    <t>Obtener seguimiento</t>
-  </si>
-  <si>
     <t>Filtro por estado de oportunidad en seguimiento</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>La aplicación debe poseer un boton donde el usuario pueda filtrar por las palabras que el ingrese.</t>
   </si>
   <si>
-    <t>La aplicación debe poseer una page de seguimiento, donde el usuario podra visualizar el seguimiento de las licitaciones.</t>
-  </si>
-  <si>
     <t>En el seguimiento, debe existir un filtro para el estado de oportunidad.</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
     <t>El dashboard debe mostrar correctamente las estadísticas de las licitaciones en seguimiento</t>
   </si>
   <si>
-    <t>El sistema debe filtrar correctamente las licitaciones en seguimiento al ingresar una palabra clave y mostrar solo los resultados coincidentes.</t>
-  </si>
-  <si>
     <t>Al acceder a la página de seguimiento, se debe mostrar la lista de todas las licitaciones que el usuario está siguiendo.</t>
   </si>
   <si>
@@ -159,16 +150,6 @@
   </si>
   <si>
     <t xml:space="preserve"> En la página de login, debería haber un botón para mostrar u ocultar la contraseña mediante íconos.</t>
-  </si>
-  <si>
-    <t>5.1. Ingresar a la página de seguimiento desde el menú de navegación principal.
-5.2. Verificar que se muestren todas las licitaciones que el usuario ha seleccionado para seguir (con sus detalles como fechas y estados).
-5.3. Hacer clic en varias licitaciones para comprobar que al seleccionarlas se navegue correctamente a la página de detalles de cada licitación.
-5.4. Verificar que la lista de licitaciones se mantenga actualizada al realizar nuevas acciones (agregar o quitar seguimientos).</t>
-  </si>
-  <si>
-    <t>1.1. Navegar por las diferentes secciones de la aplicación utilizando el BottomNavigator (Home, Seguimiento, Cuenta).
-1.2. Verificar que la navegación sea fluida y que todas las secciones se carguen correctamente sin errores de visualización.</t>
   </si>
   <si>
     <t>Visualización de datos:
@@ -184,26 +165,6 @@
 2. Verificar que se muestren todos los ítems relacionados con las diferentes oportunidades de negocio.</t>
   </si>
   <si>
-    <t>1. Navegar a la sección "Cuenta" desde el menú principal de la aplicación.
-2. Verificar que los datos del usuario, como nombre, correo electrónico, y otra información personal, se muestren correctamente.
-3. Probar editar algunos de los datos personales (como cambiar el correo electrónico) y confirmar que los cambios se guardan correctamente.
-.4. Cerrar sesión y volver a iniciar para comprobar que los datos actualizados se mantengan.
-.5. Verificar que no se muestren datos de otros usuarios por error.</t>
-  </si>
-  <si>
-    <t>1. En la sección de seguimiento, aplicar el filtro por "Estado de oportunidad" (por ejemplo, Compra Ágil, Cotizaciones).
-.2. Verificar que solo las licitaciones que corresponden a ese estado se muestren en la lista, y que el resto de las licitaciones no se visualicen.
-3. Cambiar el filtro varias veces entre los diferentes estados de oportunidad y verificar que los resultados cambian correctamente sin errores.
-4. Verificar que los datos dentro de cada licitación (como fechas y descripción) coincidan con el estado filtrado.</t>
-  </si>
-  <si>
-    <t>.1 Desde la pantalla principal, navegar a la sección de seguimiento de licitaciones.
-2. En el campo de búsqueda, ingresar palabras clave relacionadas con licitaciones que deberían estar registradas (ej. "Compra", "Proyecto").
-3. Verificar que las licitaciones que coinciden con las palabras ingresadas se filtren correctamente y se muestren sin errores.
-4. Probar búsquedas con diferentes criterios (por ejemplo, palabras incompletas o errores tipográficos) para verificar si la búsqueda es tolerante a errores o necesita mejoras.
-5. Verificar que las licitaciones no relacionadas no se muestren en los resultados.</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -225,11 +186,6 @@
   </si>
   <si>
     <t xml:space="preserve">Login exitoso: El usuario es redirigido a la página principal y se muestra un mensaje de bienvenida personalizado que indica que ha iniciado sesión correctamente.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Ingresar correo nico.vidal.m@gmail.com y contraseña válidos n1234567.
-2.diriga hacia dashboard y carguen los diferentes cuadros con datos
 </t>
   </si>
   <si>
@@ -304,6 +260,51 @@
   </si>
   <si>
     <t>CP-013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.1 Desde la pantalla principal, navegar a la sección de seguimiento de licitaciones.
+2. En el campo de búsqueda, ingresar palabras clave relacionadas con licitaciones que deberían estar registradas
+3. Verificar que las licitaciones que coinciden con las palabras ingresadas se filtren correctamente y se muestren sin errores.
+</t>
+  </si>
+  <si>
+    <t>Seguimiento</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al usuario iniciar sesión, navegar a la sección de "Seguimiento", acceder a "Oportunidades" y visualizar los ítems correspondientes.</t>
+  </si>
+  <si>
+    <t>El usuario accede a la sección de "Oportunidades" desde "Seguimiento" y puede ver los ítems relacionados.</t>
+  </si>
+  <si>
+    <t>2. Hacer clic en "Iniciar sesión".</t>
+  </si>
+  <si>
+    <t>3. Hacer clic en "Seguimiento".</t>
+  </si>
+  <si>
+    <t>4. Hacer clic en "Oportunidades".</t>
+  </si>
+  <si>
+    <t>5. Hacer clic en "Ver Ítems".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar correo y contraseña válidos .
+2.diriga hacia dashboard y carguen los diferentes cuadros con datos
+</t>
+  </si>
+  <si>
+    <t>1. Ingresar correo  y contraseña validos.
+2. Hacer clic en "Iniciar sesión".
+3. Hacer clic en "Seguimiento".
+4. Hacer clic en "Oportunidades".
+5. Hacer clic en "Ver Ítems".</t>
+  </si>
+  <si>
+    <t>Seguimiento obtenido</t>
+  </si>
+  <si>
+    <t>Busqueda funciona correctamente</t>
   </si>
 </sst>
 </file>
@@ -406,7 +407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -455,11 +456,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -504,6 +557,27 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -812,8 +886,8 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,218 +930,226 @@
     </row>
     <row r="2" spans="1:8" ht="264" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D2" s="16">
         <v>45578</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D3" s="16">
         <v>45578</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D4" s="16">
         <v>45578</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D5" s="16">
         <v>45578</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D6" s="16">
         <v>45579</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="16">
+        <v>18</v>
+      </c>
+      <c r="D7" s="19">
         <v>45581</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="23">
+        <v>45590</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="23">
+        <v>45585</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="B10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>22</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
@@ -1076,20 +1158,20 @@
     </row>
     <row r="11" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>52</v>
+        <v>41</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5" t="s">
@@ -1098,20 +1180,20 @@
     </row>
     <row r="12" spans="1:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5" t="s">
@@ -1120,36 +1202,38 @@
     </row>
     <row r="13" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="22"/>
       <c r="H13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>46</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>51</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
@@ -1158,20 +1242,20 @@
     </row>
     <row r="15" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5" t="s">

</xml_diff>

<commit_message>
Plan de pruebas 15/15
</commit_message>
<xml_diff>
--- a/Fase 2/Plan de Pruebas.xlsx
+++ b/Fase 2/Plan de Pruebas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17EA246-2087-4D1E-9374-D2D24413203D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6790660C-5CEA-40F5-ABFD-B64AC84E27FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
   <si>
     <t>Caso de Prueba</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Filtro por estado de oportunidad en seguimiento</t>
   </si>
   <si>
-    <t>Cuenta page con datos del usuario</t>
-  </si>
-  <si>
     <t>Usar BottomNavigator</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
   </si>
   <si>
     <t>Al acceder a la página de seguimiento, se debe mostrar la lista de todas las licitaciones que el usuario está siguiendo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> La página "Cuenta" debe mostrar correctamente los datos personales del usuario (nombre, email, etc.).</t>
   </si>
   <si>
     <t>Login</t>
@@ -207,9 +201,6 @@
   </si>
   <si>
     <t>Navegación y acciones exitosas</t>
-  </si>
-  <si>
-    <t>La pestaña "Cuenta" permite a los usuarios visualizar y modificar sus datos personales. Sin embargo, el campo "Correo" no es editable.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -270,14 +261,6 @@
 4. Usar el filtro para seleccionar "Ágil", "Cotizaciones" y "Convenio Marco".</t>
   </si>
   <si>
-    <t>1. Ingresar correo  y contraseña validos
-2. Hacer click en "Iniciar sesión".
-3. Hacer clickk en "Cuenta".</t>
-  </si>
-  <si>
-    <t>Datos cargados correctamente y correo no modificable.</t>
-  </si>
-  <si>
     <t>Navegar entre las pestañas "Seguimiento", "Cuenta" y "Orden de Compra".</t>
   </si>
   <si>
@@ -369,9 +352,6 @@
     <t>Olvidar/ Recuperar contraseña</t>
   </si>
   <si>
-    <t>CP-017</t>
-  </si>
-  <si>
     <t>Mostrar y ocultar la contraseña</t>
   </si>
   <si>
@@ -389,6 +369,9 @@
   </si>
   <si>
     <t xml:space="preserve">La contraseña fue mostrada al hacer clic en "Mostrar contraseña" y se ocultó al hacer clic nuevamente. </t>
+  </si>
+  <si>
+    <t>Visualizacion del dashboard obtenida correctamente</t>
   </si>
 </sst>
 </file>
@@ -512,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -539,17 +522,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -859,11 +841,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,129 +888,129 @@
     </row>
     <row r="2" spans="1:8" ht="264" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" s="7">
         <v>45578</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="7">
         <v>45578</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" s="7">
         <v>45578</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="7">
         <v>45578</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>49</v>
+        <v>23</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="D6" s="7">
         <v>45579</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>8</v>
@@ -1036,196 +1018,198 @@
     </row>
     <row r="7" spans="1:8" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="7">
         <v>45581</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="H7" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="8">
         <v>45590</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9" s="8">
         <v>45585</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D10" s="7">
         <v>45592</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D11" s="7">
         <v>45578</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="H11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="7">
+        <v>45597</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="7">
-        <v>45578</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="H12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D13" s="7">
         <v>45597</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D14" s="7">
-        <v>45597</v>
+        <v>45601</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>86</v>
@@ -1237,88 +1221,72 @@
         <v>88</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="7">
+        <v>45580</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="7">
-        <v>45601</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="H15" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>94</v>
       </c>
+      <c r="C16" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="D16" s="7">
-        <v>45580</v>
+        <v>45578</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="F16" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G16" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="99.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="7">
-        <v>45578</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1327,19 +1295,19 @@
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
       <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="3"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="3"/>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1349,17 +1317,17 @@
       <c r="G20" s="4"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="5"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1369,25 +1337,25 @@
       <c r="G22" s="5"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+    <row r="23" spans="1:10" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="11"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
@@ -1396,7 +1364,7 @@
       <c r="D25" s="11"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="12"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1479,35 +1447,15 @@
       <c r="G33" s="10"/>
       <c r="H33" s="11"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-    </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="11"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
@@ -1519,55 +1467,20 @@
       <c r="G37" s="10"/>
       <c r="H37" s="11"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="11"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-    </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="10"/>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
+      <c r="H40" s="11"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
       <c r="D41" s="11"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="11"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>

</xml_diff>